<commit_message>
fixing api loc & add session success
</commit_message>
<xml_diff>
--- a/public/file/template-soal.xlsx
+++ b/public/file/template-soal.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zack\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\tugas\public\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC49016E-8662-465E-B168-8BF129BE9542}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDBDADA4-2B83-4C12-9E0C-986EBA807224}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,17 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
-  <si>
-    <t>Semua field kolom harus diisi.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">Sistem mulai membaca data di baris ke-4, Mohon isi sesuai heading, dan tidak merubah template ini. </t>
   </si>
   <si>
-    <t>Pastikan ID Pelanggan / Nomor Meter sudah terdaftar di dalam Sistem.</t>
-  </si>
-  <si>
     <t>Nomor Soal</t>
   </si>
   <si>
@@ -66,28 +60,10 @@
     <t>Pembahasan</t>
   </si>
   <si>
-    <t>file</t>
-  </si>
-  <si>
-    <t>soal</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>swdw</t>
+    <t>Kecuali kolom Gambar, semua kolom wajib diisi!</t>
+  </si>
+  <si>
+    <t>Kosongi kolom Gambar, apabila soal terdapat Gambar bisa ditambahkan saat edit soal</t>
   </si>
 </sst>
 </file>
@@ -430,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,7 +430,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -469,7 +445,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -484,7 +460,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -499,100 +475,36 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="K4" s="4"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>1</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>20</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>